<commit_message>
`optimization test family of aircrfat ok`
</commit_message>
<xml_diff>
--- a/framework/Database/Demand/Draft_Number_of_passengers_for_15_EU_Airport_Pairs.xlsx
+++ b/framework/Database/Demand/Draft_Number_of_passengers_for_15_EU_Airport_Pairs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarc8\Documents\github\MDOAirB_base\framework\Database\Demand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2FB81A-8C92-45B4-8299-E13B7CBE0FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD47EE3-182E-49F3-83ED-54D3B3D7D482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +133,18 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -279,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,6 +318,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,8 +556,8 @@
   </sheetPr>
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -564,7 +583,7 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -587,7 +606,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
@@ -636,7 +655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
@@ -689,717 +708,717 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="15">
         <v>4509</v>
       </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
         <v>3420</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="15">
         <v>4686</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="15">
         <v>3984</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="15">
         <v>2151</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="15">
         <v>2535</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="15">
         <v>5049</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="15">
         <v>2268</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="15">
         <v>3215</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="15">
         <v>2440</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="15">
         <v>473</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="15">
         <v>2216</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="15">
         <v>2786</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="15">
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="15">
         <v>2940</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="15">
         <v>3420</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="15">
+        <v>0</v>
+      </c>
+      <c r="F6" s="15">
         <v>3337</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="15">
         <v>2996</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="15">
         <v>3738</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="15">
         <v>3545</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="15">
         <v>2044</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="15">
         <v>2549</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="15">
         <v>1925</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="15">
         <v>1801</v>
       </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
+      <c r="N6" s="15">
+        <v>0</v>
+      </c>
+      <c r="O6" s="15">
         <v>1336</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="15">
         <v>2433</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="15">
         <v>972</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="15">
         <v>2520</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="15">
         <v>4686</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="15">
         <v>3337</v>
       </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="F7" s="15">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15">
         <v>3071</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="15">
         <v>3744</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="15">
         <v>2910</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="15">
         <v>3271</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="15">
         <v>2550</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="15">
         <v>2559</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="15">
         <v>2380</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="15">
         <v>54</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="15">
         <v>1887</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="15">
         <v>2288</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="15">
         <v>616</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="15">
         <v>3132</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="15">
         <v>3984</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="15">
         <v>2996</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="15">
         <v>3071</v>
       </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="G8" s="15">
+        <v>0</v>
+      </c>
+      <c r="H8" s="15">
         <v>6969</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="15">
         <v>3402</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="15">
         <v>1501</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="15">
         <v>1498</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="15">
         <v>1832</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="15">
         <v>534</v>
       </c>
-      <c r="N8" s="2">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2">
+      <c r="N8" s="15">
+        <v>0</v>
+      </c>
+      <c r="O8" s="15">
         <v>398</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="15">
         <v>1087</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="15">
         <v>277</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="15">
         <v>2979</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="15">
         <v>2151</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="15">
         <v>3738</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="15">
         <v>3744</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="15">
         <v>6969</v>
       </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="I9" s="15">
         <v>3836</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="15">
         <v>1637</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="15">
         <v>1751</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="15">
         <v>1713</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="15">
         <v>740</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="15">
         <v>806</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="15">
         <v>897</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="15">
         <v>1037</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="15">
         <v>762</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="15">
         <v>1923</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="15">
         <v>2535</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="15">
         <v>3545</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="15">
         <v>2910</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="15">
         <v>3402</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="15">
         <v>3836</v>
       </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
+      <c r="I10" s="15">
+        <v>0</v>
+      </c>
+      <c r="J10" s="15">
         <v>553</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="15">
         <v>1435</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="15">
         <v>990</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="15">
         <v>599</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="15">
         <v>301</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="15">
         <v>728</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="15">
         <v>1020</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="Q10" s="15">
         <v>459</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="15">
         <v>2208</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="15">
         <v>5049</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="15">
         <v>2044</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="15">
         <v>3271</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="15">
         <v>1501</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="15">
         <v>1637</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="15">
         <v>553</v>
       </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
+      <c r="J11" s="15">
+        <v>0</v>
+      </c>
+      <c r="K11" s="15">
         <v>628</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="15">
         <v>783</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="15">
         <v>410</v>
       </c>
-      <c r="N11" s="2">
-        <v>0</v>
-      </c>
-      <c r="O11" s="2">
+      <c r="N11" s="15">
+        <v>0</v>
+      </c>
+      <c r="O11" s="15">
         <v>294</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="15">
         <v>521</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q11" s="15">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="15">
         <v>3237</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="15">
         <v>2268</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="15">
         <v>2549</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="15">
         <v>2550</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="15">
         <v>1498</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="15">
         <v>1751</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="15">
         <v>1435</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="15">
         <v>628</v>
       </c>
-      <c r="K12" s="2">
-        <v>0</v>
-      </c>
-      <c r="L12" s="2">
+      <c r="K12" s="15">
+        <v>0</v>
+      </c>
+      <c r="L12" s="15">
         <v>2601</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="15">
         <v>682</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="15">
         <v>456</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="15">
         <v>527</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="15">
         <v>1210</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="Q12" s="15">
         <v>914</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="15">
         <v>1875</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="15">
         <v>3215</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="15">
         <v>1925</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="15">
         <v>2559</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="15">
         <v>1832</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="15">
         <v>1713</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="15">
         <v>990</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="15">
         <v>783</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="15">
         <v>2601</v>
       </c>
-      <c r="L13" s="2">
-        <v>0</v>
-      </c>
-      <c r="M13" s="2">
+      <c r="L13" s="15">
+        <v>0</v>
+      </c>
+      <c r="M13" s="15">
         <v>1051</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="15">
         <v>524</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="15">
         <v>566</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="15">
         <v>1035</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="Q13" s="15">
         <v>303</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="15">
         <v>2004</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="15">
         <v>2440</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="15">
         <v>1801</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="15">
         <v>2380</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="15">
         <v>534</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="15">
         <v>740</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="15">
         <v>599</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="15">
         <v>410</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="15">
         <v>682</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="15">
         <v>1051</v>
       </c>
-      <c r="M14" s="2">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
+      <c r="M14" s="15">
+        <v>0</v>
+      </c>
+      <c r="N14" s="15">
+        <v>0</v>
+      </c>
+      <c r="O14" s="15">
         <v>3446</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="15">
         <v>820</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="Q14" s="15">
         <v>361</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="15">
         <v>1052</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="15">
         <v>473</v>
       </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="E15" s="15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="15">
         <v>54</v>
       </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="G15" s="15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="15">
         <v>806</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="15">
         <v>301</v>
       </c>
-      <c r="J15" s="2">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2">
+      <c r="J15" s="15">
+        <v>0</v>
+      </c>
+      <c r="K15" s="15">
         <v>456</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="15">
         <v>524</v>
       </c>
-      <c r="M15" s="2">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2">
-        <v>0</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2">
+      <c r="M15" s="15">
+        <v>0</v>
+      </c>
+      <c r="N15" s="15">
+        <v>0</v>
+      </c>
+      <c r="O15" s="15">
+        <v>0</v>
+      </c>
+      <c r="P15" s="15">
         <v>96</v>
       </c>
-      <c r="Q15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="15">
         <v>1519</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="15">
         <v>2216</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="15">
         <v>1336</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="15">
         <v>1887</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="15">
         <v>398</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="15">
         <v>897</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="15">
         <v>728</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="15">
         <v>294</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="15">
         <v>527</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="15">
         <v>566</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="15">
         <v>3446</v>
       </c>
-      <c r="N16" s="2">
-        <v>0</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0</v>
-      </c>
-      <c r="P16" s="2">
+      <c r="N16" s="15">
+        <v>0</v>
+      </c>
+      <c r="O16" s="15">
+        <v>0</v>
+      </c>
+      <c r="P16" s="15">
         <v>529</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q16" s="15">
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="15">
         <v>2565</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="15">
         <v>2786</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="15">
         <v>2433</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="15">
         <v>2288</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="15">
         <v>1087</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="15">
         <v>1037</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="15">
         <v>1020</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="15">
         <v>521</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="15">
         <v>1210</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="15">
         <v>1035</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="15">
         <v>820</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="15">
         <v>96</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="15">
         <v>529</v>
       </c>
-      <c r="P17" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="2">
+      <c r="P17" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="15">
         <v>1591</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="15">
         <v>1249</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="15">
         <v>147</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="15">
         <v>972</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="15">
         <v>616</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="15">
         <v>277</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="15">
         <v>762</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="15">
         <v>459</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="15">
         <v>58</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="15">
         <v>914</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="15">
         <v>303</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="15">
         <v>361</v>
       </c>
-      <c r="N18" s="2">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2">
+      <c r="N18" s="15">
+        <v>0</v>
+      </c>
+      <c r="O18" s="15">
         <v>156</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18" s="15">
         <v>1591</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="Q18" s="15">
         <v>0</v>
       </c>
     </row>

</xml_diff>